<commit_message>
Combine some cells in tables; Create data output for Django app, not React; Fix some small bugs
</commit_message>
<xml_diff>
--- a/backend/calculator8thFloor/fact_plan.xlsx
+++ b/backend/calculator8thFloor/fact_plan.xlsx
@@ -88,10 +88,10 @@
     <t>0.405982905982906</t>
   </si>
   <si>
-    <t>4.273504273504273</t>
-  </si>
-  <si>
-    <t>4.363675213675213</t>
+    <t>0.48846153846153845</t>
+  </si>
+  <si>
+    <t>0.5786324786324787</t>
   </si>
 </sst>
 </file>
@@ -498,7 +498,7 @@
         <v>20</v>
       </c>
       <c r="G3">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H3">
         <v>600</v>
@@ -519,7 +519,7 @@
         <v>21</v>
       </c>
       <c r="N3">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:14">
@@ -542,7 +542,7 @@
         <v>20</v>
       </c>
       <c r="G4">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H4">
         <v>600</v>
@@ -563,7 +563,7 @@
         <v>21</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:14">
@@ -630,7 +630,7 @@
         <v>22</v>
       </c>
       <c r="G6">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H6">
         <v>600</v>
@@ -651,7 +651,7 @@
         <v>23</v>
       </c>
       <c r="N6">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:14">
@@ -662,7 +662,7 @@
         <v>1170</v>
       </c>
       <c r="C7">
-        <v>10000</v>
+        <v>1143</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -674,7 +674,7 @@
         <v>24</v>
       </c>
       <c r="G7">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="H7">
         <v>600</v>
@@ -683,7 +683,7 @@
         <v>1</v>
       </c>
       <c r="J7">
-        <v>10211</v>
+        <v>1354</v>
       </c>
       <c r="K7">
         <v>2</v>
@@ -695,7 +695,7 @@
         <v>25</v>
       </c>
       <c r="N7">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>